<commit_message>
DC-cambios en el excel de la rubrica de los juegos
</commit_message>
<xml_diff>
--- a/juego.xlsx
+++ b/juego.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\universidad\gamificacion\proyecto_final\soundFlow_back\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\universidad\9no semestre\gamificacion\proyecto-final\soundFlow_back\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F3A9C2B-DDB3-4283-A42D-E5D056C624D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C8381A-B352-406E-993F-AE632AFCBFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{819E379E-6A1A-4BE4-AE0A-9ED3A8BFE4ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Juego de asociación de notas musicales. Asocia cada nota musical con su nombre correspondiente.</t>
   </si>
@@ -117,6 +117,27 @@
   </si>
   <si>
     <t>escala_Do</t>
+  </si>
+  <si>
+    <t>Encuentra la tónica de una escala mayor. Observa una escala mayor y selecciona la nota que actúa como tónica.</t>
+  </si>
+  <si>
+    <t>Juego de completar escalas mayores. Completa las notas faltantes en una escala mayor dada.</t>
+  </si>
+  <si>
+    <t>Construcción de escalas menores naturales. Coloca las notas en el orden correcto para formar una escala menor natural dada.</t>
+  </si>
+  <si>
+    <t>Juego de tonos y semitonos en escalas menores. Mueve las notas en un teclado virtual para crear patrones de tonos y semitonos en escalas menores naturales.</t>
+  </si>
+  <si>
+    <t>Do,Mi,Sol,Si</t>
+  </si>
+  <si>
+    <t>Dom</t>
+  </si>
+  <si>
+    <t>Do,Re,Mib,Fa,Sol,Lab,Sib</t>
   </si>
 </sst>
 </file>
@@ -152,19 +173,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,46 +506,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D83341-32BC-415E-85CB-487CCEF32E05}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -530,28 +554,28 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -560,28 +584,28 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="4">
         <v>3</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
       <c r="C14" t="s">
         <v>11</v>
       </c>
@@ -590,28 +614,28 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>14</v>
       </c>
@@ -620,28 +644,28 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="4">
         <v>5</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
       <c r="C24" t="s">
         <v>17</v>
       </c>
@@ -650,28 +674,28 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="4">
         <v>6</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
       <c r="C29" t="s">
         <v>20</v>
       </c>
@@ -680,28 +704,28 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="4">
         <v>7</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
       <c r="C34" t="s">
         <v>20</v>
       </c>
@@ -710,28 +734,28 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="4">
         <v>8</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
       <c r="C39" t="s">
         <v>25</v>
       </c>
@@ -740,272 +764,290 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="4">
         <v>9</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="1"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="1"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="1"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="1"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="4">
         <v>10</v>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
         <v>11</v>
       </c>
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="B52" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="3"/>
+      <c r="C54" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
         <v>12</v>
       </c>
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="B57" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
         <v>13</v>
       </c>
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="1"/>
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="3"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="1"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="3"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="1"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="3"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="A67" s="4">
         <v>14</v>
       </c>
-      <c r="B67" s="1"/>
+      <c r="B67" s="3"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-      <c r="B68" s="1"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="3"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
-      <c r="B69" s="1"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="3"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
-      <c r="B70" s="1"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="3"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-      <c r="B71" s="1"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="3"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="A72" s="4">
         <v>15</v>
       </c>
-      <c r="B72" s="1"/>
+      <c r="B72" s="3"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
-      <c r="B73" s="1"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="3"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
-      <c r="B74" s="1"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="3"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2"/>
-      <c r="B75" s="1"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="3"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
-      <c r="B76" s="1"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="3"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="A77" s="4">
         <v>16</v>
       </c>
-      <c r="B77" s="1"/>
+      <c r="B77" s="3"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="1"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="3"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="1"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="3"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="1"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="3"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="1"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="3"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="A82" s="4">
         <v>17</v>
       </c>
-      <c r="B82" s="1"/>
+      <c r="B82" s="3"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
-      <c r="B83" s="1"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="3"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
-      <c r="B84" s="1"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="3"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2"/>
-      <c r="B85" s="1"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="3"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
-      <c r="B86" s="1"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="3"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="A87" s="4">
         <v>18</v>
       </c>
-      <c r="B87" s="1"/>
+      <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-      <c r="B88" s="1"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="3"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-      <c r="B89" s="1"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="3"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="B90" s="1"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="3"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
-      <c r="B91" s="1"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="3"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="A92" s="4">
         <v>19</v>
       </c>
-      <c r="B92" s="1"/>
+      <c r="B92" s="3"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-      <c r="B93" s="1"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="3"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-      <c r="B94" s="1"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="3"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2"/>
-      <c r="B95" s="1"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2"/>
-      <c r="B96" s="1"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A77:A81"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A12:A16"/>
     <mergeCell ref="A92:A96"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B22:B26"/>
@@ -1022,13 +1064,21 @@
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="B92:B96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
DC - actualización de excel con las rubricas de juego
</commit_message>
<xml_diff>
--- a/juego.xlsx
+++ b/juego.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\universidad\9no semestre\gamificacion\proyecto-final\soundFlow_back\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\universidad\gamificacion\proyecto_final\soundFlow_back\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C8381A-B352-406E-993F-AE632AFCBFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7767A58-5336-4F01-9C85-88170D72AE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{819E379E-6A1A-4BE4-AE0A-9ED3A8BFE4ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Juego de asociación de notas musicales. Asocia cada nota musical con su nombre correspondiente.</t>
   </si>
@@ -138,6 +138,24 @@
   </si>
   <si>
     <t>Do,Re,Mib,Fa,Sol,Lab,Sib</t>
+  </si>
+  <si>
+    <t>Rem</t>
+  </si>
+  <si>
+    <t>Re:T,Mi:S,Fa:T,Sol:T,La:S,Sib:T,Do:T</t>
+  </si>
+  <si>
+    <t>Reconocimiento auditivo de escalas menores naturales. Escucha una escala menor natural y selecciona su tonalidad correcta.</t>
+  </si>
+  <si>
+    <t>son_esca_do_me</t>
+  </si>
+  <si>
+    <t>Escala_do_me</t>
+  </si>
+  <si>
+    <t>Encuentra la tónica de una escala menor. Observa una escala menor y selecciona la nota que actúa como tónica.</t>
   </si>
 </sst>
 </file>
@@ -182,13 +200,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,13 +524,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D83341-32BC-415E-85CB-487CCEF32E05}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -535,17 +553,17 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="5"/>
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -555,27 +573,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="5"/>
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -585,27 +603,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="3"/>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>3</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="3"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="3"/>
+      <c r="B14" s="5"/>
       <c r="C14" t="s">
         <v>11</v>
       </c>
@@ -615,27 +633,27 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="5"/>
       <c r="C19" t="s">
         <v>14</v>
       </c>
@@ -645,27 +663,27 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>5</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="3"/>
+      <c r="B24" s="5"/>
       <c r="C24" t="s">
         <v>17</v>
       </c>
@@ -675,27 +693,27 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="3"/>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>6</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
+      <c r="B29" s="5"/>
       <c r="C29" t="s">
         <v>20</v>
       </c>
@@ -705,27 +723,27 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="3"/>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>7</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="3"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="3"/>
+      <c r="B34" s="5"/>
       <c r="C34" t="s">
         <v>20</v>
       </c>
@@ -735,27 +753,27 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="3"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="3"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>8</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="3"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="3"/>
+      <c r="B39" s="5"/>
       <c r="C39" t="s">
         <v>25</v>
       </c>
@@ -765,27 +783,27 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="3"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="3"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>9</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="3"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="3"/>
+      <c r="B44" s="5"/>
       <c r="C44" t="s">
         <v>5</v>
       </c>
@@ -795,27 +813,27 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="3"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="3"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>10</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
-      <c r="B48" s="3"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="3"/>
+      <c r="B49" s="5"/>
       <c r="C49" t="s">
         <v>31</v>
       </c>
@@ -825,27 +843,27 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="3"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
-      <c r="B51" s="3"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>11</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
-      <c r="B53" s="3"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
-      <c r="B54" s="3"/>
+      <c r="B54" s="5"/>
       <c r="C54" t="s">
         <v>32</v>
       </c>
@@ -855,199 +873,221 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
-      <c r="B55" s="3"/>
+      <c r="B55" s="5"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="3"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>12</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
-      <c r="B58" s="3"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
-      <c r="B59" s="3"/>
+      <c r="B59" s="5"/>
+      <c r="C59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
-      <c r="B60" s="3"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
-      <c r="B61" s="3"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>13</v>
       </c>
-      <c r="B62" s="3"/>
+      <c r="B62" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
-      <c r="B63" s="3"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
-      <c r="B64" s="3"/>
+      <c r="B64" s="5"/>
+      <c r="C64" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
-      <c r="B65" s="3"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
-      <c r="B66" s="3"/>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>14</v>
       </c>
-      <c r="B67" s="3"/>
+      <c r="B67" s="5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
-      <c r="B68" s="3"/>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
-      <c r="B69" s="3"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
-      <c r="B70" s="3"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
-      <c r="B71" s="3"/>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>15</v>
       </c>
-      <c r="B72" s="3"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
-      <c r="B73" s="3"/>
+      <c r="B73" s="5"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
-      <c r="B74" s="3"/>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
-      <c r="B75" s="3"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
-      <c r="B76" s="3"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>16</v>
       </c>
-      <c r="B77" s="3"/>
+      <c r="B77" s="5"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
-      <c r="B78" s="3"/>
+      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
-      <c r="B79" s="3"/>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
-      <c r="B80" s="3"/>
+      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
-      <c r="B81" s="3"/>
+      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>17</v>
       </c>
-      <c r="B82" s="3"/>
+      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
-      <c r="B83" s="3"/>
+      <c r="B83" s="5"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
-      <c r="B84" s="3"/>
+      <c r="B84" s="5"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
-      <c r="B85" s="3"/>
+      <c r="B85" s="5"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
-      <c r="B86" s="3"/>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>18</v>
       </c>
-      <c r="B87" s="3"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
-      <c r="B88" s="3"/>
+      <c r="B88" s="5"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
-      <c r="B89" s="3"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
-      <c r="B90" s="3"/>
+      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
-      <c r="B91" s="3"/>
+      <c r="B91" s="5"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>19</v>
       </c>
-      <c r="B92" s="3"/>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
-      <c r="B93" s="3"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
-      <c r="B94" s="3"/>
+      <c r="B94" s="5"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
-      <c r="B95" s="3"/>
+      <c r="B95" s="5"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
-      <c r="B96" s="3"/>
+      <c r="B96" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="B87:B91"/>
     <mergeCell ref="A92:A96"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B22:B26"/>
@@ -1064,21 +1104,15 @@
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A77:A81"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A12:A16"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="B92:B96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
DC-cambios en el excel de la rubrica de los juegos : finalizado
</commit_message>
<xml_diff>
--- a/juego.xlsx
+++ b/juego.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\universidad\gamificacion\proyecto_final\soundFlow_back\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\universidad\9no semestre\gamificacion\proyecto-final\soundFlow_back\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7767A58-5336-4F01-9C85-88170D72AE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2456F01-71B4-459F-8292-DB43C4BD6AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{819E379E-6A1A-4BE4-AE0A-9ED3A8BFE4ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Juego de asociación de notas musicales. Asocia cada nota musical con su nombre correspondiente.</t>
   </si>
@@ -156,6 +156,60 @@
   </si>
   <si>
     <t>Encuentra la tónica de una escala menor. Observa una escala menor y selecciona la nota que actúa como tónica.</t>
+  </si>
+  <si>
+    <t>Re,Mi,Fa,Sol,La,Sib,Do</t>
+  </si>
+  <si>
+    <t>Re</t>
+  </si>
+  <si>
+    <t>Juego de completar escalas menores. Completa las notas faltantes en una escala menor dada.</t>
+  </si>
+  <si>
+    <t>Identificación de notas alteradas en el pentagrama. Observa las notas en un pentagrama y marca las notas que están alteradas (sostenidas o bemoles).</t>
+  </si>
+  <si>
+    <t>Do, Do#,Re,Re#,La,La#</t>
+  </si>
+  <si>
+    <t>Do#,Re#,La#</t>
+  </si>
+  <si>
+    <t>Construcción de escalas mayores con notas alteradas. Agrega las notas alteradas necesarias para formar escalas mayores en diferentes tonalidades.</t>
+  </si>
+  <si>
+    <t>mi, fa#, sol#, la, si, do#, y re#</t>
+  </si>
+  <si>
+    <t>Mi,la,si</t>
+  </si>
+  <si>
+    <t>Juego de reconocimiento auditivo de notas alteradas. Escucha una nota y selecciona si es sostenida o bemol.</t>
+  </si>
+  <si>
+    <t>sound_sol_sost</t>
+  </si>
+  <si>
+    <t>Sol#</t>
+  </si>
+  <si>
+    <t>sound_mi_b</t>
+  </si>
+  <si>
+    <t>Mib</t>
+  </si>
+  <si>
+    <t>Encuentra la nota alterada. Observa una escala mayor y selecciona la nota que está alterada.</t>
+  </si>
+  <si>
+    <t>Do,Re,Sol -&gt; dom</t>
+  </si>
+  <si>
+    <t>Re,Mi,Fa#,Sol,La,Si,Do#,Re</t>
+  </si>
+  <si>
+    <t>Fa#,Do#</t>
   </si>
 </sst>
 </file>
@@ -203,10 +257,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D83341-32BC-415E-85CB-487CCEF32E05}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,20 +604,20 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -572,28 +626,28 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -602,28 +656,28 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="5">
         <v>3</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14" t="s">
         <v>11</v>
       </c>
@@ -632,28 +686,28 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="5">
         <v>4</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
       <c r="C19" t="s">
         <v>14</v>
       </c>
@@ -662,28 +716,28 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="5">
         <v>5</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="4"/>
       <c r="C24" t="s">
         <v>17</v>
       </c>
@@ -692,28 +746,28 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="5">
         <v>6</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="4"/>
       <c r="C29" t="s">
         <v>20</v>
       </c>
@@ -722,28 +776,28 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="5">
         <v>7</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="4"/>
       <c r="C34" t="s">
         <v>20</v>
       </c>
@@ -752,28 +806,28 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37" s="5">
         <v>8</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="4"/>
       <c r="C39" t="s">
         <v>25</v>
       </c>
@@ -782,28 +836,28 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="A42" s="5">
         <v>9</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="4"/>
       <c r="C44" t="s">
         <v>5</v>
       </c>
@@ -812,28 +866,28 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="A47" s="5">
         <v>10</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="4"/>
       <c r="C49" t="s">
         <v>31</v>
       </c>
@@ -842,28 +896,28 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="A52" s="5">
         <v>11</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="4"/>
       <c r="C54" t="s">
         <v>32</v>
       </c>
@@ -872,28 +926,28 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="A57" s="5">
         <v>12</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="4"/>
       <c r="C59" t="s">
         <v>34</v>
       </c>
@@ -902,28 +956,28 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="A62" s="5">
         <v>13</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="4"/>
       <c r="C64" t="s">
         <v>37</v>
       </c>
@@ -931,163 +985,211 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="5"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="5"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="4"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="4"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
         <v>14</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="5"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="5"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="5"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="5"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="4"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="4"/>
+      <c r="C69" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="4"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="4"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
         <v>15</v>
       </c>
-      <c r="B72" s="5"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="5"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="5"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="5"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="5"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+      <c r="B72" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="4"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="4"/>
+      <c r="C74" t="s">
+        <v>55</v>
+      </c>
+      <c r="D74" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="4"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="4"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
         <v>16</v>
       </c>
-      <c r="B77" s="5"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="5"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="5"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="5"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="5"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
+      <c r="B77" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="4"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+      <c r="B79" s="4"/>
+      <c r="C79" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="B80" s="4"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="4"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="5">
         <v>17</v>
       </c>
-      <c r="B82" s="5"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="5"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="5"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="5"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="5"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
+      <c r="B82" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="B83" s="4"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+      <c r="B84" s="4"/>
+      <c r="C84" t="s">
+        <v>48</v>
+      </c>
+      <c r="D84" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="4"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="4"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
         <v>18</v>
       </c>
-      <c r="B87" s="5"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="5"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="5"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="5"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="5"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+      <c r="B87" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="4"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
+      <c r="B89" s="4"/>
+      <c r="C89" t="s">
+        <v>50</v>
+      </c>
+      <c r="D89" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="4"/>
+      <c r="C90" t="s">
+        <v>52</v>
+      </c>
+      <c r="D90" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+      <c r="B91" s="4"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
         <v>19</v>
       </c>
-      <c r="B92" s="5"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="5"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="5"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="5"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="5"/>
+      <c r="B92" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+      <c r="B93" s="4"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
+      <c r="B94" s="4"/>
+      <c r="C94" t="s">
+        <v>56</v>
+      </c>
+      <c r="D94" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="4"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A77:A81"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B42:B46"/>
     <mergeCell ref="A92:A96"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B22:B26"/>
@@ -1104,15 +1206,19 @@
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B67:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>